<commit_message>
Change to embeddings only workflow
</commit_message>
<xml_diff>
--- a/to_code_sample.xlsx
+++ b/to_code_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonysneed/Library/CloudStorage/Dropbox/Distribute/Finance/Code/Auto Coding Program/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonysneed/Source/transaction-autocoder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD595D6-892E-C148-BE96-3B8CBF733EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46C0702-2578-AD43-9954-6DFA45D45F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="26120" windowHeight="15740" xr2:uid="{8F118B2E-D109-4184-83AE-4FEF54688670}"/>
   </bookViews>
@@ -914,7 +914,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>